<commit_message>
layout alterado, inserido mais uma coluna na linha três
</commit_message>
<xml_diff>
--- a/dre.xlsx
+++ b/dre.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bde24405a60f0cea/Área de Trabalho/Dre1920/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bde24405a60f0cea/Área de Trabalho/AnalysisFinance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="670" documentId="13_ncr:1_{2C6D1234-065A-42EB-AE37-D47D7FD9CE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A2B45A5-CD8D-479E-89B8-85C6B79154D0}"/>
+  <xr:revisionPtr revIDLastSave="672" documentId="13_ncr:1_{2C6D1234-065A-42EB-AE37-D47D7FD9CE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B93F73A9-A6D6-44F2-BCAE-0D5ED25B346E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="808" xr2:uid="{5DF10B22-BEAD-48A1-9E42-2634BFE0BF64}"/>
   </bookViews>
@@ -240,7 +240,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,13 +272,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -321,14 +314,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,11 +391,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -421,54 +406,48 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,7 +460,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +482,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -812,7 +787,7 @@
   <dimension ref="A1:BE29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,185 +846,185 @@
     <col min="53" max="53" width="13.33203125" customWidth="1"/>
     <col min="54" max="54" width="17.88671875" customWidth="1"/>
     <col min="55" max="55" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="37.88671875" customWidth="1"/>
     <col min="57" max="57" width="53.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:57" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="W1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="X1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="Y1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="Z1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AA1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AB1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AC1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AD1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AE1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AF1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AG1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AH1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AI1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AJ1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AK1" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="AL1" s="21" t="s">
+      <c r="AL1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AM1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="21" t="s">
+      <c r="AN1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="21" t="s">
+      <c r="AO1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AP1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AQ1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AR1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="AS1" s="21" t="s">
+      <c r="AS1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="21" t="s">
+      <c r="AT1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="AU1" s="21" t="s">
+      <c r="AU1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="AV1" s="21" t="s">
+      <c r="AV1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="21" t="s">
+      <c r="AW1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AX1" s="21" t="s">
+      <c r="AX1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="AY1" s="21" t="s">
+      <c r="AY1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="AZ1" s="21" t="s">
+      <c r="AZ1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="BA1" s="21" t="s">
+      <c r="BA1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="BB1" s="21" t="s">
+      <c r="BB1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="BC1" s="21" t="s">
+      <c r="BC1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="BD1" s="21" t="s">
+      <c r="BD1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BE1" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A2" s="26">
+      <c r="A2" s="24">
         <v>2018</v>
       </c>
       <c r="B2" s="3">
@@ -1073,7 +1048,7 @@
       <c r="H2" s="3">
         <v>15754</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="23">
         <v>4897843</v>
       </c>
       <c r="J2" s="3">
@@ -1097,7 +1072,7 @@
       <c r="P2" s="3">
         <v>-42719</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="Q2" s="23">
         <v>2309468</v>
       </c>
       <c r="R2" s="3">
@@ -1117,7 +1092,7 @@
         <v>-10808</v>
       </c>
       <c r="X2" s="3"/>
-      <c r="Y2" s="25">
+      <c r="Y2" s="23">
         <v>356221</v>
       </c>
       <c r="Z2" s="7">
@@ -1206,7 +1181,7 @@
       </c>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
@@ -1230,7 +1205,7 @@
       <c r="H3" s="3">
         <v>16925</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="23">
         <v>5068774</v>
       </c>
       <c r="J3" s="3">
@@ -1254,7 +1229,7 @@
       <c r="P3" s="3">
         <v>-26616</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3" s="23">
         <v>2352984</v>
       </c>
       <c r="R3" s="3">
@@ -1276,7 +1251,7 @@
       <c r="X3" s="3">
         <v>-501796</v>
       </c>
-      <c r="Y3" s="25">
+      <c r="Y3" s="23">
         <v>1033084</v>
       </c>
       <c r="Z3" s="7">
@@ -1367,7 +1342,7 @@
       </c>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3">
@@ -1391,7 +1366,7 @@
       <c r="H4" s="3">
         <v>13338</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="23">
         <v>3936227</v>
       </c>
       <c r="J4" s="3">
@@ -1415,7 +1390,7 @@
       <c r="P4" s="3">
         <v>-33839</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="23">
         <v>1748384</v>
       </c>
       <c r="R4" s="3">
@@ -1437,7 +1412,7 @@
       <c r="X4" s="3">
         <v>-524946</v>
       </c>
-      <c r="Y4" s="25">
+      <c r="Y4" s="23">
         <v>-164238</v>
       </c>
       <c r="Z4" s="7">
@@ -1524,7 +1499,7 @@
       </c>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3">
@@ -1548,7 +1523,7 @@
       <c r="H5" s="3">
         <v>17599</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <v>4978232</v>
       </c>
       <c r="J5" s="3">
@@ -1572,7 +1547,7 @@
       <c r="P5" s="3">
         <v>-46129</v>
       </c>
-      <c r="Q5" s="25">
+      <c r="Q5" s="23">
         <v>2224318</v>
       </c>
       <c r="R5" s="3">
@@ -1596,7 +1571,7 @@
       <c r="X5" s="3">
         <v>-554641</v>
       </c>
-      <c r="Y5" s="25">
+      <c r="Y5" s="23">
         <v>92798</v>
       </c>
       <c r="Z5" s="7">
@@ -1683,7 +1658,7 @@
       </c>
     </row>
     <row r="6" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
@@ -1707,7 +1682,7 @@
       <c r="H6" s="3">
         <v>21693</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <v>5926177</v>
       </c>
       <c r="J6" s="3">
@@ -1731,7 +1706,7 @@
       <c r="P6" s="3">
         <v>-49381</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6" s="23">
         <v>2850268</v>
       </c>
       <c r="R6" s="3">
@@ -1755,7 +1730,7 @@
       <c r="X6" s="11">
         <v>-641887</v>
       </c>
-      <c r="Y6" s="25">
+      <c r="Y6" s="23">
         <v>268180</v>
       </c>
       <c r="Z6" s="7">
@@ -1846,7 +1821,7 @@
       </c>
     </row>
     <row r="7" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
@@ -1870,7 +1845,7 @@
       <c r="H7" s="3">
         <v>26025</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <v>6362725</v>
       </c>
       <c r="J7" s="3">
@@ -1894,7 +1869,7 @@
       <c r="P7" s="3">
         <v>-86303</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7" s="23">
         <v>3166759</v>
       </c>
       <c r="R7" s="3">
@@ -1918,7 +1893,7 @@
       <c r="X7" s="14">
         <v>-707827</v>
       </c>
-      <c r="Y7" s="25">
+      <c r="Y7" s="23">
         <v>394446</v>
       </c>
       <c r="Z7" s="17">
@@ -2028,7 +2003,7 @@
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="24"/>
+      <c r="C10" s="22"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
       <c r="AR10" s="4"/>
@@ -2038,7 +2013,7 @@
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="24"/>
+      <c r="C11" s="22"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AR11" s="4"/>
@@ -2074,28 +2049,28 @@
       <c r="AW15" s="5"/>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="AR16" s="30"/>
+      <c r="AR16" s="28"/>
       <c r="AW16" s="5"/>
     </row>
     <row r="17" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B17" s="29"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="26"/>
     </row>
     <row r="19" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B19" s="29"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="26"/>
     </row>
     <row r="21" spans="2:44" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
     <row r="23" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B23" s="29"/>
-      <c r="C23" s="28"/>
-      <c r="AR23" s="30"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="26"/>
+      <c r="AR23" s="28"/>
     </row>
     <row r="25" spans="2:44" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="28"/>
+      <c r="C25" s="26"/>
     </row>
     <row r="27" spans="2:44" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>

</xml_diff>